<commit_message>
Done formatting Now testing colors
</commit_message>
<xml_diff>
--- a/res/ID exercises.xlsx
+++ b/res/ID exercises.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Study\Applab\Code\Applab\Python-graphs\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rick Dijkstra\Documents\Study\Applab\Moment2Moment\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F824B1D-3ABF-4AD7-976F-748196A1FB71}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A763A61-0BB8-421D-B861-0E14ED098C6E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -423,10 +423,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Blad1"/>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,8 +888,13 @@
         <v>1474967</v>
       </c>
     </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2151774</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:F26">
+  <conditionalFormatting sqref="A1:F26 A27">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added creating long files. Updated boundary checker
</commit_message>
<xml_diff>
--- a/res/ID exercises.xlsx
+++ b/res/ID exercises.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rick Dijkstra\Documents\Study\Applab\Moment2Moment\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A763A61-0BB8-421D-B861-0E14ED098C6E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B0FE0E-9775-451A-B245-0E68A804B929}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -423,10 +423,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Blad1"/>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,11 +888,6 @@
         <v>1474967</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>2151774</v>
-      </c>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:F26 A27">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>

</xml_diff>